<commit_message>
Repaired and upgraded linking and mapping tools
</commit_message>
<xml_diff>
--- a/assets/linking.xlsx
+++ b/assets/linking.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\FPS\QSS\CLOSER\USP\05 Metadata Enhancement\Bundles\TOOLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CLOSER-dev\PyCharm\Bundler\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="linking.txt" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Demographics</t>
   </si>
@@ -413,181 +413,25 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>slist!A2</f>
         <v>0</v>
       </c>
       <c r="B1">
-        <f>IFERROR(INDEX(CV!A1:A14,MATCH(linking!$B2,CV!B1:B14,0)),0)</f>
+        <f>slist!B2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>slist!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>IFERROR(INDEX(CV!A2:A15,MATCH(linking!$B3,CV!B2:B15,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>slist!A4</f>
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <f>IFERROR(INDEX(CV!A3:A16,MATCH(linking!$B4,CV!B3:B16,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>slist!A5</f>
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <f>IFERROR(INDEX(CV!A4:A17,MATCH(linking!$B5,CV!B4:B17,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>slist!A6</f>
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <f>IFERROR(INDEX(CV!A5:A18,MATCH(linking!$B6,CV!B5:B18,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>slist!A7</f>
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <f>IFERROR(INDEX(CV!A6:A19,MATCH(linking!$B7,CV!B6:B19,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f>slist!A8</f>
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <f>IFERROR(INDEX(CV!A7:A20,MATCH(linking!$B8,CV!B7:B20,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f>slist!A9</f>
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <f>IFERROR(INDEX(CV!A8:A21,MATCH(linking!$B9,CV!B8:B21,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>slist!A10</f>
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <f>IFERROR(INDEX(CV!A9:A22,MATCH(linking!$B10,CV!B9:B22,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>slist!A11</f>
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <f>IFERROR(INDEX(CV!A10:A23,MATCH(linking!$B11,CV!B10:B23,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f>slist!A12</f>
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <f>IFERROR(INDEX(CV!A11:A24,MATCH(linking!$B12,CV!B11:B24,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>slist!A13</f>
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <f>IFERROR(INDEX(CV!A12:A25,MATCH(linking!$B13,CV!B12:B25,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>slist!A14</f>
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <f>IFERROR(INDEX(CV!A13:A26,MATCH(linking!$B14,CV!B13:B26,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>slist!A15</f>
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <f>IFERROR(INDEX(CV!A14:A27,MATCH(linking!$B15,CV!B14:B27,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>slist!A16</f>
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <f>IFERROR(INDEX(CV!A15:A28,MATCH(linking!$B16,CV!B15:B28,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>slist!A17</f>
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <f>IFERROR(INDEX(CV!A16:A29,MATCH(linking!$B17,CV!B16:B29,0)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>slist!A18</f>
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <f>IFERROR(INDEX(CV!A17:A30,MATCH(linking!$B18,CV!B17:B30,0)),0)</f>
+      <c r="C1">
+        <f>IFERROR(INDEX(CV!$A$1:$A$14,MATCH(linking!$B2,CV!$B$1:$B$14,0)),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -601,19 +445,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="B1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -628,7 +472,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,10 +599,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,154 +621,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>slist!A2</f>
+        <f>slist!B2</f>
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>slist!A3</f>
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>slist!A4</f>
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>slist!A5</f>
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>slist!A6</f>
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f>slist!A7</f>
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f>slist!A8</f>
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>slist!A9</f>
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>slist!A10</f>
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f>slist!A11</f>
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>slist!A12</f>
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>slist!A13</f>
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>slist!A14</f>
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>slist!A15</f>
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>slist!A16</f>
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>slist!A17</f>
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>slist!A18</f>
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -938,7 +638,7 @@
           <x14:formula1>
             <xm:f>CV!$B$1:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B18</xm:sqref>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>